<commit_message>
feb 07, 2025, commit #4
</commit_message>
<xml_diff>
--- a/reductions.xlsx
+++ b/reductions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/506594a149b35854/Desktop/Development Projects/ISO 9001 Audit Time Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10485E5118603A5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61A907C1-BA3E-4E41-B2C0-6BF5027E1489}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC10485E5118603A5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F82A5D-8B63-4D9E-81B2-FC74CC9AD8B8}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
     </row>
     <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>

</xml_diff>